<commit_message>
Atualização geral na análise de dados
</commit_message>
<xml_diff>
--- a/data/production/tree_classifier_production.xlsx
+++ b/data/production/tree_classifier_production.xlsx
@@ -535,7 +535,7 @@
         <v>9.6</v>
       </c>
       <c r="L2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -576,7 +576,7 @@
         <v>9.5</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9.675000000000001</v>
+        <v>10.7</v>
       </c>
       <c r="B4" t="n">
         <v>0.67</v>
@@ -605,13 +605,13 @@
         <v>34</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9991374999999998</v>
+        <v>1.0004</v>
       </c>
       <c r="I4" t="n">
         <v>3.28</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8625</v>
+        <v>0.98</v>
       </c>
       <c r="K4" t="n">
         <v>9.9</v>
@@ -658,10 +658,10 @@
         <v>9.800000000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -696,10 +696,10 @@
         <v>0.6</v>
       </c>
       <c r="K6" t="n">
-        <v>10.5</v>
+        <v>10.6</v>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>0.083</v>
       </c>
       <c r="F7" t="n">
-        <v>34.125</v>
+        <v>35</v>
       </c>
       <c r="G7" t="n">
         <v>72</v>
@@ -740,7 +740,7 @@
         <v>9.4</v>
       </c>
       <c r="L7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -766,7 +766,7 @@
         <v>23</v>
       </c>
       <c r="G8" t="n">
-        <v>125.875</v>
+        <v>147</v>
       </c>
       <c r="H8" t="n">
         <v>0.99636</v>
@@ -781,7 +781,7 @@
         <v>9.699999999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
@@ -822,7 +822,7 @@
         <v>10</v>
       </c>
       <c r="L9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -863,7 +863,7 @@
         <v>9.800000000000001</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -901,10 +901,10 @@
         <v>0.66</v>
       </c>
       <c r="K11" t="n">
-        <v>10.5</v>
+        <v>10.9</v>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>

</xml_diff>